<commit_message>
fix MTD bug and add rw log page issue
</commit_message>
<xml_diff>
--- a/source/Product/template/rw_log.xlsx
+++ b/source/Product/template/rw_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>類別</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,6 +39,14 @@
   </si>
   <si>
     <t>工號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defect code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -46,7 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -59,6 +67,15 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -95,7 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -378,21 +395,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="3" max="5" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,6 +420,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>